<commit_message>
Remove Specfic File Name
</commit_message>
<xml_diff>
--- a/DriveSummaryPython.xlsx
+++ b/DriveSummaryPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveDashboardPython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="11_DA39029DC6B1C53613CB09DD21CE172C5C824D09" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{72EA6F94-D0B4-40D6-B4D2-20E35C8DEE1F}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_DA393215BE7DC4D5877D6BC0435F12371CE042DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B37FFF26-4627-478F-AE38-7E613E9F8E2B}"/>
   <bookViews>
-    <workbookView xWindow="-4140" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -134,9 +134,6 @@
   </si>
   <si>
     <t>Report Date</t>
-  </si>
-  <si>
-    <t>2025/05/30</t>
   </si>
   <si>
     <t>Last Month's Status</t>
@@ -572,7 +569,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -765,26 +762,18 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Blue" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -2809,23 +2798,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
-<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
-  <bag type="Checkbox"/>
-  <bag type="XFControls">
-    <bagId k="CellControl">0</bagId>
-  </bag>
-  <bag type="XFComplement">
-    <bagId k="XFControls">1</bagId>
-  </bag>
-  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
-    <a k="MappedFeaturePropertyBags">
-      <bagId>2</bagId>
-    </a>
-  </bag>
-</FeaturePropertyBags>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3262,8 +3234,8 @@
   </sheetPr>
   <dimension ref="B2:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3286,29 +3258,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="28" width="8.85546875" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="32" width="8.85546875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="69" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Stefan May 2025</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="71"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -3320,7 +3292,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>May 2025</v>
+        <v>June 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -3328,21 +3300,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="68"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="68"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -3357,11 +3329,11 @@
       </c>
       <c r="F6" s="6">
         <f>J9</f>
-        <v>1572.799</v>
+        <v>1614.9259999999999</v>
       </c>
       <c r="G6" s="17">
         <f>J33</f>
-        <v>1492</v>
+        <v>1542</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
@@ -3407,11 +3379,11 @@
       </c>
       <c r="F7" s="6">
         <f>F6/J23*J22</f>
-        <v>1625.2256333333335</v>
+        <v>1614.9259999999999</v>
       </c>
       <c r="G7" s="6">
         <f>G6/J23*J22</f>
-        <v>1541.7333333333333</v>
+        <v>1542</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -3455,11 +3427,11 @@
       </c>
       <c r="F8" s="65">
         <f>F6/J23</f>
-        <v>52.426633333333335</v>
+        <v>52.094387096774192</v>
       </c>
       <c r="G8" s="65">
         <f>G6/J23</f>
-        <v>49.733333333333334</v>
+        <v>49.741935483870968</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
@@ -3506,13 +3478,13 @@
       </c>
       <c r="G9" s="63">
         <f>50*J24 + IF(J22&lt;30,(30-J22)*G8,0)</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="6">
-        <v>1572.799</v>
+        <v>1614.9259999999999</v>
       </c>
       <c r="L9" s="11">
         <v>600</v>
@@ -3575,7 +3547,7 @@
         <f>SUM(C6:C10)</f>
         <v>2650</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="68"/>
@@ -3644,7 +3616,7 @@
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="72" t="b">
+      <c r="C13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -3681,8 +3653,8 @@
       <c r="I14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="58" t="s">
-        <v>31</v>
+      <c r="J14" s="58">
+        <v>45808</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
@@ -3693,11 +3665,11 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="67" t="str">
+      <c r="N15" s="66" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
       <c r="P15" s="68"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
@@ -3722,7 +3694,7 @@
     </row>
     <row r="17" spans="9:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>15</v>
@@ -3742,9 +3714,11 @@
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I18" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J18" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="J18" s="1">
+        <v>50</v>
+      </c>
       <c r="N18" s="1">
         <v>300</v>
       </c>
@@ -3767,8 +3741,8 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="67" t="s">
-        <v>34</v>
+      <c r="I20" s="66" t="s">
+        <v>33</v>
       </c>
       <c r="J20" s="68"/>
       <c r="N20" s="1">
@@ -3819,11 +3793,11 @@
     </row>
     <row r="23" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I23" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N23" s="1">
         <v>1800</v>
@@ -3837,32 +3811,32 @@
     </row>
     <row r="24" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I24" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" s="54">
         <f>J22-J23</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I25" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25" s="56">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>150</v>
       </c>
-      <c r="M25" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
+      <c r="M25" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="68"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" s="57">
         <f>MAX(0,C9-J25)</f>
@@ -3875,18 +3849,18 @@
         <v>10</v>
       </c>
       <c r="O26" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="P26" s="16" t="s">
+      <c r="Q26" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="Q26" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I27" s="54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J27" s="54">
         <f t="array" ref="J27">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J26))</f>
@@ -3905,12 +3879,12 @@
         <v>0.05</v>
       </c>
       <c r="Q27" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I28" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J28" s="62">
         <f>IF(ISBLANK(J18),ROUND(50-J6/J23,0),J18)</f>
@@ -3929,12 +3903,12 @@
         <v>0.1</v>
       </c>
       <c r="Q28" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I29" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J29" s="61">
         <f>J8</f>
@@ -3953,12 +3927,12 @@
         <v>0.2</v>
       </c>
       <c r="Q29" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I30" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30" s="60">
         <f>J29*J28</f>
@@ -3977,16 +3951,16 @@
         <v>0.35</v>
       </c>
       <c r="Q30" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I31" s="53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M31" s="47">
         <v>2500</v>
@@ -4001,16 +3975,16 @@
         <v>0.5</v>
       </c>
       <c r="Q31" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I32" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
-        <v>1292</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
@@ -4019,28 +3993,28 @@
       </c>
       <c r="J33" s="6">
         <f>J30+J32</f>
-        <v>1492</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
-        <v>2642</v>
+        <v>2692</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="I11:J11"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
     <cfRule type="expression" dxfId="29" priority="1">
@@ -4099,8 +4073,8 @@
   </sheetPr>
   <dimension ref="B2:AC34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4113,39 +4087,39 @@
     <col min="6" max="6" width="11.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="2.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="12" max="14" width="9.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="10.5703125" style="2" hidden="1" customWidth="1"/>
-    <col min="16" max="17" width="9.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" style="2" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="2.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="2.7109375" style="2" customWidth="1"/>
+    <col min="12" max="14" width="9.7109375" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="2" customWidth="1"/>
+    <col min="16" max="17" width="9.7109375" style="2" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="28" width="8.85546875" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="32" width="8.85546875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="69" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Christiaan May 2025</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="71"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -4157,7 +4131,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>May 2025</v>
+        <v>June 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -4165,21 +4139,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="68"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="68"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -4194,17 +4168,17 @@
       </c>
       <c r="F6" s="6">
         <f>J9</f>
-        <v>1500</v>
+        <v>1496.702</v>
       </c>
       <c r="G6" s="17">
         <f>J33</f>
-        <v>1392</v>
+        <v>1550</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>9</v>
@@ -4244,17 +4218,17 @@
       </c>
       <c r="F7" s="6">
         <f>F6/J23*J22</f>
-        <v>1660.7142857142856</v>
+        <v>1496.702</v>
       </c>
       <c r="G7" s="6">
         <f>G6/J23*J22</f>
-        <v>1541.1428571428571</v>
+        <v>1550</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L7" s="11">
         <v>0</v>
@@ -4285,24 +4259,24 @@
       </c>
       <c r="C8" s="6">
         <f>300-J7</f>
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="65">
         <f>F6/J23</f>
-        <v>53.571428571428569</v>
+        <v>48.280709677419352</v>
       </c>
       <c r="G8" s="65">
         <f>G6/J23</f>
-        <v>49.714285714285715</v>
+        <v>50</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L8" s="11">
         <v>300</v>
@@ -4332,24 +4306,24 @@
       </c>
       <c r="C9" s="6">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>250</v>
+        <v>300</v>
       </c>
       <c r="E9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="63" t="str">
+      <c r="F9" s="63">
         <f>IF(J27&gt;=M13, "Unlimited", J27-F6)</f>
-        <v>Unlimited</v>
+        <v>302.298</v>
       </c>
       <c r="G9" s="63">
         <f>50*J24 + IF(J22&lt;30,(30-J22)*G8,0)</f>
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="1">
-        <v>1500</v>
+        <v>1496.702</v>
       </c>
       <c r="L9" s="11">
         <v>600</v>
@@ -4410,9 +4384,9 @@
       </c>
       <c r="C11" s="6">
         <f>SUM(C6:C10)</f>
-        <v>2650</v>
-      </c>
-      <c r="I11" s="67" t="s">
+        <v>2682</v>
+      </c>
+      <c r="I11" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="68"/>
@@ -4481,14 +4455,14 @@
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="72" t="b">
+      <c r="C13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L13" s="12">
         <v>1800</v>
@@ -4519,7 +4493,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="58">
-        <v>45805</v>
+        <v>45808</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
@@ -4530,11 +4504,11 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="67" t="str">
+      <c r="N15" s="66" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
       <c r="P15" s="68"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
@@ -4559,7 +4533,7 @@
     </row>
     <row r="17" spans="9:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>15</v>
@@ -4579,7 +4553,7 @@
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1"/>
       <c r="N18" s="1">
@@ -4604,8 +4578,8 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="67" t="s">
-        <v>34</v>
+      <c r="I20" s="66" t="s">
+        <v>33</v>
       </c>
       <c r="J20" s="68"/>
       <c r="N20" s="1">
@@ -4656,11 +4630,11 @@
     </row>
     <row r="23" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I23" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N23" s="1">
         <v>1800</v>
@@ -4674,36 +4648,36 @@
     </row>
     <row r="24" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I24" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" s="54">
         <f>J22-J23</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I25" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25" s="56">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>150</v>
-      </c>
-      <c r="M25" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
+        <v>182</v>
+      </c>
+      <c r="M25" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="68"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" s="57">
         <f>MAX(0,C9-J25)</f>
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="M26" s="16" t="s">
         <v>9</v>
@@ -4712,22 +4686,22 @@
         <v>10</v>
       </c>
       <c r="O26" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="P26" s="16" t="s">
+      <c r="Q26" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="Q26" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I27" s="54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J27" s="54">
         <f t="array" ref="J27">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J26))</f>
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="M27" s="34">
         <v>0</v>
@@ -4742,12 +4716,12 @@
         <v>0.05</v>
       </c>
       <c r="Q27" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I28" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J28" s="62">
         <f>IF(ISBLANK(J18),ROUND(50-J6/J23,0),J18)</f>
@@ -4766,16 +4740,16 @@
         <v>0.1</v>
       </c>
       <c r="Q28" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I29" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J29" s="61">
         <f>J8</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M29" s="40">
         <v>1600</v>
@@ -4790,16 +4764,16 @@
         <v>0.2</v>
       </c>
       <c r="Q29" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I30" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30" s="60">
         <f>J29*J28</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="M30" s="43">
         <v>2200</v>
@@ -4814,16 +4788,16 @@
         <v>0.35</v>
       </c>
       <c r="Q30" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I31" s="53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="M31" s="47">
         <v>2500</v>
@@ -4838,16 +4812,16 @@
         <v>0.5</v>
       </c>
       <c r="Q31" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I32" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
-        <v>1192</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
@@ -4856,28 +4830,28 @@
       </c>
       <c r="J33" s="6">
         <f>J30+J32</f>
-        <v>1392</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
-        <v>2542</v>
+        <v>2732</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="I11:J11"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -4960,29 +4934,29 @@
     <col min="19" max="19" width="2.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="28" width="8.85546875" style="2" customWidth="1"/>
-    <col min="29" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="32" width="8.85546875" style="2" customWidth="1"/>
+    <col min="33" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="69" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Derrick May 2025</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="71"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -4994,7 +4968,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>May 2025</v>
+        <v>June 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -5002,21 +4976,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="68"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="68"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -5249,7 +5223,7 @@
         <f>SUM(C6:C10)</f>
         <v>2650</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="68"/>
@@ -5318,14 +5292,14 @@
       <c r="B13" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="72" t="b">
+      <c r="C13" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L13" s="12">
         <v>1800</v>
@@ -5367,11 +5341,11 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="67" t="str">
+      <c r="N15" s="66" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
       <c r="P15" s="68"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
@@ -5396,7 +5370,7 @@
     </row>
     <row r="17" spans="9:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J17" s="6" t="s">
         <v>15</v>
@@ -5416,7 +5390,7 @@
     </row>
     <row r="18" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I18" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J18" s="1"/>
       <c r="N18" s="1">
@@ -5441,8 +5415,8 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="67" t="s">
-        <v>34</v>
+      <c r="I20" s="66" t="s">
+        <v>33</v>
       </c>
       <c r="J20" s="68"/>
       <c r="N20" s="1">
@@ -5493,7 +5467,7 @@
     </row>
     <row r="23" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I23" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
@@ -5511,7 +5485,7 @@
     </row>
     <row r="24" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I24" s="51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J24" s="54">
         <f>J22-J23</f>
@@ -5520,23 +5494,23 @@
     </row>
     <row r="25" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I25" s="53" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25" s="56">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>150</v>
       </c>
-      <c r="M25" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
+      <c r="M25" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="68"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26" s="57">
         <f>MAX(0,C9-J25)</f>
@@ -5549,18 +5523,18 @@
         <v>10</v>
       </c>
       <c r="O26" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="P26" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="P26" s="16" t="s">
+      <c r="Q26" s="16" t="s">
         <v>41</v>
-      </c>
-      <c r="Q26" s="16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="27" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I27" s="54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J27" s="54">
         <f t="array" ref="J27">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J26))</f>
@@ -5579,12 +5553,12 @@
         <v>0.05</v>
       </c>
       <c r="Q27" s="36" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I28" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J28" s="62">
         <f>IF(ISBLANK(J18),ROUND(50-J6/J23,0),J18)</f>
@@ -5603,12 +5577,12 @@
         <v>0.1</v>
       </c>
       <c r="Q28" s="39" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I29" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J29" s="61">
         <f>J8</f>
@@ -5627,12 +5601,12 @@
         <v>0.2</v>
       </c>
       <c r="Q29" s="42" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I30" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="J30" s="60">
         <f>J29*J28</f>
@@ -5651,12 +5625,12 @@
         <v>0.35</v>
       </c>
       <c r="Q30" s="46" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I31" s="53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
@@ -5675,12 +5649,12 @@
         <v>0.5</v>
       </c>
       <c r="Q31" s="50" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I32" s="54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
@@ -5698,7 +5672,7 @@
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I34" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
@@ -5707,14 +5681,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="I11:J11"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Fix: Report Dates Function Created (#1)
</commit_message>
<xml_diff>
--- a/DriveSummaryPython.xlsx
+++ b/DriveSummaryPython.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveDashboardPython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_DA393215BE7DC4D5877D6BC0435F12371CE042DE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B37FFF26-4627-478F-AE38-7E613E9F8E2B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_DB39829FABD98605447DF927DA0E9D26FCE77716" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3235,7 +3235,7 @@
   <dimension ref="B2:AC34"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,8 +3258,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="32" width="8.85546875" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="35" width="8.85546875" style="2" customWidth="1"/>
+    <col min="36" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4073,8 +4073,8 @@
   </sheetPr>
   <dimension ref="B2:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4097,8 +4097,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="32" width="8.85546875" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="35" width="8.85546875" style="2" customWidth="1"/>
+    <col min="36" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4322,7 +4322,7 @@
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="6">
         <v>1496.702</v>
       </c>
       <c r="L9" s="11">
@@ -4934,8 +4934,8 @@
     <col min="19" max="19" width="2.7109375" style="2" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="32" width="8.85546875" style="2" customWidth="1"/>
-    <col min="33" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="35" width="8.85546875" style="2" customWidth="1"/>
+    <col min="36" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CSV files from old DQ Mapper Dashboard - using the New dashboard from the next commit onwards
</commit_message>
<xml_diff>
--- a/DriveSummaryPython.xlsx
+++ b/DriveSummaryPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveDashboardPython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="11_1A3F6660C07985319E12EDDF673E1B693402463A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD8C3C3C-3CCC-43AD-8C86-EDD487D898CA}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="11_DB39929DDFC906A18BDB1C1AE1FF92D54060565A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E40CFE83-1D57-40FE-8657-3A69EF504D65}"/>
   <bookViews>
-    <workbookView xWindow="-4140" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10275" yWindow="-16200" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="59">
   <si>
     <t>Description</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>Derrick</t>
+  </si>
+  <si>
+    <t>Missed</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>Speed 15 is only</t>
+  </si>
+  <si>
+    <t>dws Drive pen</t>
   </si>
 </sst>
 </file>
@@ -216,7 +228,7 @@
     <numFmt numFmtId="164" formatCode="[$R-1C09]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +268,14 @@
       <color theme="1"/>
       <name val="72 Monospace"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -569,7 +589,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -762,18 +782,22 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Blue" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -3235,7 +3259,7 @@
   <dimension ref="B2:AC34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:K35"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3258,29 +3282,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="39" width="8.85546875" style="2" customWidth="1"/>
-    <col min="40" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="42" width="8.85546875" style="2" customWidth="1"/>
+    <col min="43" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="69" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan June 2025</v>
-      </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+        <v>Drive Summary Stefan July 2025</v>
+      </c>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="71"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -3300,21 +3324,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="68"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="68"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -3322,25 +3346,25 @@
       </c>
       <c r="C6" s="6">
         <f>MIN(1500, IF($C$13,G7,G6+G9))</f>
-        <v>1444</v>
+        <v>1500</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="6">
         <f>J9</f>
-        <v>1731.587</v>
+        <v>1052.94</v>
       </c>
       <c r="G6" s="17">
         <f>J33</f>
-        <v>1444</v>
+        <v>762</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1">
-        <f>46+8</f>
-        <v>54</v>
+        <f>45-9</f>
+        <v>36</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>9</v>
@@ -3380,11 +3404,11 @@
       </c>
       <c r="F7" s="6">
         <f>F6/J23*J22</f>
-        <v>1731.587</v>
+        <v>2040.0712500000002</v>
       </c>
       <c r="G7" s="6">
         <f>G6/J23*J22</f>
-        <v>1444</v>
+        <v>1476.375</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -3428,11 +3452,11 @@
       </c>
       <c r="F8" s="65">
         <f>F6/J23</f>
-        <v>57.719566666666665</v>
+        <v>65.808750000000003</v>
       </c>
       <c r="G8" s="65">
         <f>G6/J23</f>
-        <v>48.133333333333333</v>
+        <v>47.625</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
@@ -3468,24 +3492,24 @@
       </c>
       <c r="C9" s="6">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="63">
+      <c r="F9" s="63" t="str">
         <f>IF(J27&gt;=M13, "Unlimited", J27-F6)</f>
-        <v>67.413000000000011</v>
+        <v>Unlimited</v>
       </c>
       <c r="G9" s="63">
         <f>50*J24 + IF(J22&lt;30,(30-J22)*G8,0)</f>
-        <v>0</v>
+        <v>750</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="6">
-        <v>1731.587</v>
+        <v>1052.94</v>
       </c>
       <c r="L9" s="11">
         <v>600</v>
@@ -3546,9 +3570,9 @@
       </c>
       <c r="C11" s="6">
         <f>SUM(C6:C10)</f>
-        <v>2544</v>
-      </c>
-      <c r="I11" s="67" t="s">
+        <v>2700</v>
+      </c>
+      <c r="I11" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="68"/>
@@ -3655,7 +3679,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="58">
-        <v>45838</v>
+        <v>45854</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
@@ -3666,11 +3690,11 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="67" t="str">
+      <c r="N15" s="66" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
       <c r="P15" s="68"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
@@ -3693,7 +3717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="9:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="5:17" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I17" s="6" t="s">
         <v>31</v>
       </c>
@@ -3713,7 +3737,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="18" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I18" s="6" t="s">
         <v>32</v>
       </c>
@@ -3730,7 +3754,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="19" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
       <c r="N19" s="1">
         <v>600</v>
       </c>
@@ -3741,8 +3765,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="67" t="s">
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="I20" s="66" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="68"/>
@@ -3756,7 +3780,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I21" s="16" t="s">
         <v>0</v>
       </c>
@@ -3773,14 +3797,14 @@
         <v>300</v>
       </c>
     </row>
-    <row r="22" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I22" s="52" t="str">
         <f>_xlfn.CONCAT("Days ",TEXT(J14, "mmm yyyy"))</f>
-        <v>Days Jun 2025</v>
+        <v>Days Jul 2025</v>
       </c>
       <c r="J22" s="55">
         <f>DAY(EOMONTH(J14, 0))</f>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N22" s="1">
         <v>1500</v>
@@ -3792,13 +3816,13 @@
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I23" s="52" t="s">
         <v>34</v>
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="N23" s="1">
         <v>1800</v>
@@ -3810,38 +3834,38 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I24" s="51" t="s">
         <v>35</v>
       </c>
       <c r="J24" s="54">
         <f>J22-J23</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="9:17" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I25" s="53" t="s">
         <v>36</v>
       </c>
       <c r="J25" s="56">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>44</v>
-      </c>
-      <c r="M25" s="67" t="s">
+        <v>200</v>
+      </c>
+      <c r="M25" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="68"/>
     </row>
-    <row r="26" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">
         <v>38</v>
       </c>
       <c r="J26" s="57">
         <f>MAX(0,C9-J25)</f>
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="M26" s="16" t="s">
         <v>9</v>
@@ -3859,13 +3883,13 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I27" s="54" t="s">
         <v>42</v>
       </c>
       <c r="J27" s="54">
         <f t="array" ref="J27">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J26))</f>
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="M27" s="34">
         <v>0</v>
@@ -3883,7 +3907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I28" s="62" t="s">
         <v>32</v>
       </c>
@@ -3907,7 +3931,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I29" s="61" t="s">
         <v>45</v>
       </c>
@@ -3931,7 +3955,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I30" s="60" t="s">
         <v>47</v>
       </c>
@@ -3955,13 +3979,16 @@
         <v>48</v>
       </c>
     </row>
-    <row r="31" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E31" s="72" t="s">
+        <v>55</v>
+      </c>
       <c r="I31" s="53" t="s">
         <v>49</v>
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="M31" s="47">
         <v>2500</v>
@@ -3979,43 +4006,61 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="9:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+      <c r="F32" s="2">
+        <v>3</v>
+      </c>
       <c r="I32" s="54" t="s">
         <v>51</v>
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
-        <v>1396</v>
-      </c>
-    </row>
-    <row r="33" spans="9:10" x14ac:dyDescent="0.25">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="2">
+        <v>3</v>
+      </c>
       <c r="I33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J33" s="6">
         <f>J30+J32</f>
-        <v>1444</v>
-      </c>
-    </row>
-    <row r="34" spans="9:10" x14ac:dyDescent="0.25">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="34" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E34" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="73">
+        <v>-9</v>
+      </c>
       <c r="I34" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
-        <v>2544</v>
+        <v>1962</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="I11:J11"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
     <cfRule type="expression" dxfId="29" priority="1">
@@ -4059,10 +4104,10 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="43" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="43" orientation="landscape"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -4098,29 +4143,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="39" width="8.85546875" style="2" customWidth="1"/>
-    <col min="40" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="42" width="8.85546875" style="2" customWidth="1"/>
+    <col min="43" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="69" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Christiaan May 2025</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="71"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -4140,21 +4185,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="68"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="68"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -4387,7 +4432,7 @@
         <f>SUM(C6:C10)</f>
         <v>2682</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="68"/>
@@ -4505,11 +4550,11 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="67" t="str">
+      <c r="N15" s="66" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
       <c r="P15" s="68"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
@@ -4579,7 +4624,7 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="67" t="s">
+      <c r="I20" s="66" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="68"/>
@@ -4664,12 +4709,12 @@
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>182</v>
       </c>
-      <c r="M25" s="67" t="s">
+      <c r="M25" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="68"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
@@ -4845,14 +4890,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="I11:J11"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
     <cfRule type="expression" dxfId="19" priority="1">
@@ -4935,29 +4980,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="39" width="8.85546875" style="2" customWidth="1"/>
-    <col min="40" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="42" width="8.85546875" style="2" customWidth="1"/>
+    <col min="43" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="str">
+      <c r="B2" s="69" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Derrick May 2025</v>
       </c>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
       <c r="E2" s="71"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
       <c r="E3" s="71"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -4977,21 +5022,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="67" t="s">
+      <c r="I5" s="66" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="68"/>
-      <c r="L5" s="67" t="s">
+      <c r="L5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="O5" s="67"/>
+      <c r="P5" s="67"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="68"/>
-      <c r="AB5" s="66"/>
-      <c r="AC5" s="66"/>
+      <c r="AB5" s="70"/>
+      <c r="AC5" s="70"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -5224,7 +5269,7 @@
         <f>SUM(C6:C10)</f>
         <v>2600</v>
       </c>
-      <c r="I11" s="67" t="s">
+      <c r="I11" s="66" t="s">
         <v>25</v>
       </c>
       <c r="J11" s="68"/>
@@ -5342,11 +5387,11 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="67" t="str">
+      <c r="N15" s="66" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="69"/>
+      <c r="O15" s="67"/>
       <c r="P15" s="68"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
@@ -5416,7 +5461,7 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="67" t="s">
+      <c r="I20" s="66" t="s">
         <v>33</v>
       </c>
       <c r="J20" s="68"/>
@@ -5501,12 +5546,12 @@
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>100</v>
       </c>
-      <c r="M25" s="67" t="s">
+      <c r="M25" s="66" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
+      <c r="N25" s="67"/>
+      <c r="O25" s="67"/>
+      <c r="P25" s="67"/>
       <c r="Q25" s="68"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
@@ -5682,14 +5727,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="M25:Q25"/>
-    <mergeCell ref="I11:J11"/>
     <mergeCell ref="AB5:AC5"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="N15:P15"/>
     <mergeCell ref="B2:G3"/>
     <mergeCell ref="L5:R5"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M25:Q25"/>
+    <mergeCell ref="I11:J11"/>
   </mergeCells>
   <conditionalFormatting sqref="B11:C12">
     <cfRule type="expression" dxfId="9" priority="1">

</xml_diff>

<commit_message>
Updated script to work with the new DQ Mapper detailed report data.
</commit_message>
<xml_diff>
--- a/DriveSummaryPython.xlsx
+++ b/DriveSummaryPython.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveDashboardPython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_DB39929DDFC906A18BDB1C1AE1FF92D54060565A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E40CFE83-1D57-40FE-8657-3A69EF504D65}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_F3BD3F85E4EDE6FC0854EB8D43DF9FB6B8225A81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E20906-125E-4993-BEB0-ED5F8549470F}"/>
   <bookViews>
-    <workbookView xWindow="10275" yWindow="-16200" windowWidth="14610" windowHeight="16305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="55">
   <si>
     <t>Description</t>
   </si>
@@ -206,18 +206,6 @@
   </si>
   <si>
     <t>Derrick</t>
-  </si>
-  <si>
-    <t>Missed</t>
-  </si>
-  <si>
-    <t>Speed</t>
-  </si>
-  <si>
-    <t>Speed 15 is only</t>
-  </si>
-  <si>
-    <t>dws Drive pen</t>
   </si>
 </sst>
 </file>
@@ -782,6 +770,10 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -794,10 +786,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Blue" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
@@ -3259,7 +3247,7 @@
   <dimension ref="B2:AC34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3282,29 +3270,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="42" width="8.85546875" style="2" customWidth="1"/>
-    <col min="43" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="43" width="8.85546875" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="71" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan July 2025</v>
-      </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+        <v>Drive Summary Stefan August 2025</v>
+      </c>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -3316,7 +3304,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>July 2025</v>
+        <v>September 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -3324,21 +3312,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="66" t="s">
+      <c r="I5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="68"/>
-      <c r="L5" s="66" t="s">
+      <c r="J5" s="70"/>
+      <c r="L5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="68"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="70"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="70"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="72"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -3353,18 +3341,17 @@
       </c>
       <c r="F6" s="6">
         <f>J9</f>
-        <v>1052.94</v>
+        <v>905.95864092000011</v>
       </c>
       <c r="G6" s="17">
         <f>J33</f>
-        <v>762</v>
+        <v>1513</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1">
-        <f>45-9</f>
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>9</v>
@@ -3404,11 +3391,11 @@
       </c>
       <c r="F7" s="6">
         <f>F6/J23*J22</f>
-        <v>2040.0712500000002</v>
+        <v>905.95864092000011</v>
       </c>
       <c r="G7" s="6">
         <f>G6/J23*J22</f>
-        <v>1476.375</v>
+        <v>1513</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -3452,17 +3439,17 @@
       </c>
       <c r="F8" s="65">
         <f>F6/J23</f>
-        <v>65.808750000000003</v>
+        <v>29.224472287741939</v>
       </c>
       <c r="G8" s="65">
         <f>G6/J23</f>
-        <v>47.625</v>
+        <v>48.806451612903224</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="1">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="L8" s="11">
         <v>300</v>
@@ -3503,13 +3490,13 @@
       </c>
       <c r="G9" s="63">
         <f>50*J24 + IF(J22&lt;30,(30-J22)*G8,0)</f>
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="6">
-        <v>1052.94</v>
+        <v>905.95864092000011</v>
       </c>
       <c r="L9" s="11">
         <v>600</v>
@@ -3572,10 +3559,10 @@
         <f>SUM(C6:C10)</f>
         <v>2700</v>
       </c>
-      <c r="I11" s="66" t="s">
+      <c r="I11" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="68"/>
+      <c r="J11" s="70"/>
       <c r="L11" s="11">
         <v>1200</v>
       </c>
@@ -3679,7 +3666,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="58">
-        <v>45854</v>
+        <v>45900</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
@@ -3690,12 +3677,12 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="66" t="str">
+      <c r="N15" s="68" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="67"/>
-      <c r="P15" s="68"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="70"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
@@ -3742,7 +3729,7 @@
         <v>32</v>
       </c>
       <c r="J18" s="1">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="N18" s="1">
         <v>300</v>
@@ -3766,10 +3753,10 @@
       </c>
     </row>
     <row r="20" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="66" t="s">
+      <c r="I20" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="68"/>
+      <c r="J20" s="70"/>
       <c r="N20" s="1">
         <v>900</v>
       </c>
@@ -3800,7 +3787,7 @@
     <row r="22" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I22" s="52" t="str">
         <f>_xlfn.CONCAT("Days ",TEXT(J14, "mmm yyyy"))</f>
-        <v>Days Jul 2025</v>
+        <v>Days Aug 2025</v>
       </c>
       <c r="J22" s="55">
         <f>DAY(EOMONTH(J14, 0))</f>
@@ -3822,7 +3809,7 @@
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="N23" s="1">
         <v>1800</v>
@@ -3840,7 +3827,7 @@
       </c>
       <c r="J24" s="54">
         <f>J22-J23</f>
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="5:17" x14ac:dyDescent="0.25">
@@ -3851,13 +3838,13 @@
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>200</v>
       </c>
-      <c r="M25" s="66" t="s">
+      <c r="M25" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="68"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="70"/>
     </row>
     <row r="26" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">
@@ -3913,7 +3900,7 @@
       </c>
       <c r="J28" s="62">
         <f>IF(ISBLANK(J18),ROUND(50-J6/J23,0),J18)</f>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M28" s="37">
         <v>800</v>
@@ -3937,7 +3924,7 @@
       </c>
       <c r="J29" s="61">
         <f>J8</f>
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="M29" s="40">
         <v>1600</v>
@@ -3961,7 +3948,7 @@
       </c>
       <c r="J30" s="60">
         <f>J29*J28</f>
-        <v>48</v>
+        <v>1029</v>
       </c>
       <c r="M30" s="43">
         <v>2200</v>
@@ -3980,15 +3967,13 @@
       </c>
     </row>
     <row r="31" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E31" s="72" t="s">
-        <v>55</v>
-      </c>
+      <c r="E31" s="66"/>
       <c r="I31" s="53" t="s">
         <v>49</v>
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="M31" s="47">
         <v>2500</v>
@@ -4007,48 +3992,32 @@
       </c>
     </row>
     <row r="32" spans="5:17" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="2">
-        <v>3</v>
-      </c>
       <c r="I32" s="54" t="s">
         <v>51</v>
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
-        <v>714</v>
+        <v>484</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
-        <v>57</v>
-      </c>
-      <c r="F33" s="2">
-        <v>3</v>
-      </c>
       <c r="I33" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J33" s="6">
         <f>J30+J32</f>
-        <v>762</v>
+        <v>1513</v>
       </c>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E34" s="72" t="s">
-        <v>58</v>
-      </c>
-      <c r="F34" s="73">
-        <v>-9</v>
-      </c>
+      <c r="E34" s="66"/>
+      <c r="F34" s="67"/>
       <c r="I34" s="1" t="s">
         <v>52</v>
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
-        <v>1962</v>
+        <v>2713</v>
       </c>
     </row>
   </sheetData>
@@ -4143,29 +4112,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="42" width="8.85546875" style="2" customWidth="1"/>
-    <col min="43" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="43" width="8.85546875" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="71" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Christiaan May 2025</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -4177,7 +4146,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>July 2025</v>
+        <v>September 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -4185,21 +4154,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="66" t="s">
+      <c r="I5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="68"/>
-      <c r="L5" s="66" t="s">
+      <c r="J5" s="70"/>
+      <c r="L5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="68"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="70"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="70"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="72"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -4432,10 +4401,10 @@
         <f>SUM(C6:C10)</f>
         <v>2682</v>
       </c>
-      <c r="I11" s="66" t="s">
+      <c r="I11" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="68"/>
+      <c r="J11" s="70"/>
       <c r="L11" s="11">
         <v>1200</v>
       </c>
@@ -4550,12 +4519,12 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="66" t="str">
+      <c r="N15" s="68" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="67"/>
-      <c r="P15" s="68"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="70"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
@@ -4624,10 +4593,10 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="66" t="s">
+      <c r="I20" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="68"/>
+      <c r="J20" s="70"/>
       <c r="N20" s="1">
         <v>900</v>
       </c>
@@ -4709,13 +4678,13 @@
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>182</v>
       </c>
-      <c r="M25" s="66" t="s">
+      <c r="M25" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="68"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="70"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">
@@ -4980,29 +4949,29 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="42" width="8.85546875" style="2" customWidth="1"/>
-    <col min="43" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="43" width="8.85546875" style="2" customWidth="1"/>
+    <col min="44" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="str">
+      <c r="B2" s="71" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
         <v>Drive Summary Derrick May 2025</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
       <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="13"/>
     </row>
     <row r="5" spans="2:29" x14ac:dyDescent="0.25">
@@ -5014,7 +4983,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>July 2025</v>
+        <v>September 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -5022,21 +4991,21 @@
       <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I5" s="66" t="s">
+      <c r="I5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="68"/>
-      <c r="L5" s="66" t="s">
+      <c r="J5" s="70"/>
+      <c r="L5" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="67"/>
-      <c r="O5" s="67"/>
-      <c r="P5" s="67"/>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="68"/>
-      <c r="AB5" s="70"/>
-      <c r="AC5" s="70"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+      <c r="R5" s="70"/>
+      <c r="AB5" s="72"/>
+      <c r="AC5" s="72"/>
     </row>
     <row r="6" spans="2:29" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -5269,10 +5238,10 @@
         <f>SUM(C6:C10)</f>
         <v>2600</v>
       </c>
-      <c r="I11" s="66" t="s">
+      <c r="I11" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="68"/>
+      <c r="J11" s="70"/>
       <c r="L11" s="11">
         <v>1200</v>
       </c>
@@ -5387,12 +5356,12 @@
       <c r="J15" s="6">
         <v>300</v>
       </c>
-      <c r="N15" s="66" t="str">
+      <c r="N15" s="68" t="str">
         <f>_xlfn.CONCAT("Distance Points for ",J17)</f>
         <v>Distance Points for Diamond</v>
       </c>
-      <c r="O15" s="67"/>
-      <c r="P15" s="68"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="70"/>
       <c r="V15" s="9"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
@@ -5461,10 +5430,10 @@
       </c>
     </row>
     <row r="20" spans="9:17" x14ac:dyDescent="0.25">
-      <c r="I20" s="66" t="s">
+      <c r="I20" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="68"/>
+      <c r="J20" s="70"/>
       <c r="N20" s="1">
         <v>900</v>
       </c>
@@ -5546,13 +5515,13 @@
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
         <v>100</v>
       </c>
-      <c r="M25" s="66" t="s">
+      <c r="M25" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="N25" s="67"/>
-      <c r="O25" s="67"/>
-      <c r="P25" s="67"/>
-      <c r="Q25" s="68"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="70"/>
     </row>
     <row r="26" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I26" s="55" t="s">

</xml_diff>

<commit_message>
Updated for Stefan September and family
</commit_message>
<xml_diff>
--- a/DriveSummaryPython.xlsx
+++ b/DriveSummaryPython.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveDashboardPython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_F3BD3F85E4EDE6FC0854EB8D43DF9FB6B8225A81" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92E20906-125E-4993-BEB0-ED5F8549470F}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_827B1A28EC29E536E13BCA8A87AF1E0808C0452D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03019B32-D834-48E8-BB07-1E79455A56B0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2910" yWindow="-16320" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="1" r:id="rId1"/>
@@ -3270,14 +3270,14 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="43" width="8.85546875" style="2" customWidth="1"/>
-    <col min="44" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="44" width="8.85546875" style="2" customWidth="1"/>
+    <col min="45" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan August 2025</v>
+        <v>Drive Summary Stefan September 2025</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
@@ -3304,7 +3304,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>September 2025</v>
+        <v>October 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -3334,24 +3334,24 @@
       </c>
       <c r="C6" s="6">
         <f>MIN(1500, IF($C$13,G7,G6+G9))</f>
-        <v>1500</v>
+        <v>1420</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="6">
         <f>J9</f>
-        <v>905.95864092000011</v>
+        <v>1601.64</v>
       </c>
       <c r="G6" s="17">
         <f>J33</f>
-        <v>1513</v>
+        <v>1420</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>9</v>
@@ -3391,11 +3391,11 @@
       </c>
       <c r="F7" s="6">
         <f>F6/J23*J22</f>
-        <v>905.95864092000011</v>
+        <v>1601.64</v>
       </c>
       <c r="G7" s="6">
         <f>G6/J23*J22</f>
-        <v>1513</v>
+        <v>1420</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
@@ -3439,17 +3439,17 @@
       </c>
       <c r="F8" s="65">
         <f>F6/J23</f>
-        <v>29.224472287741939</v>
+        <v>53.388000000000005</v>
       </c>
       <c r="G8" s="65">
         <f>G6/J23</f>
-        <v>48.806451612903224</v>
+        <v>47.333333333333336</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="1">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="L8" s="11">
         <v>300</v>
@@ -3479,14 +3479,14 @@
       </c>
       <c r="C9" s="6">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="E9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="63" t="str">
+      <c r="F9" s="63">
         <f>IF(J27&gt;=M13, "Unlimited", J27-F6)</f>
-        <v>Unlimited</v>
+        <v>197.3599999999999</v>
       </c>
       <c r="G9" s="63">
         <f>50*J24 + IF(J22&lt;30,(30-J22)*G8,0)</f>
@@ -3496,7 +3496,7 @@
         <v>2</v>
       </c>
       <c r="J9" s="6">
-        <v>905.95864092000011</v>
+        <v>1601.64</v>
       </c>
       <c r="L9" s="11">
         <v>600</v>
@@ -3557,7 +3557,7 @@
       </c>
       <c r="C11" s="6">
         <f>SUM(C6:C10)</f>
-        <v>2700</v>
+        <v>2520</v>
       </c>
       <c r="I11" s="68" t="s">
         <v>25</v>
@@ -3666,7 +3666,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="58">
-        <v>45900</v>
+        <v>45930</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
@@ -3787,11 +3787,11 @@
     <row r="22" spans="5:17" x14ac:dyDescent="0.25">
       <c r="I22" s="52" t="str">
         <f>_xlfn.CONCAT("Days ",TEXT(J14, "mmm yyyy"))</f>
-        <v>Days Aug 2025</v>
+        <v>Days Sept 2025</v>
       </c>
       <c r="J22" s="55">
         <f>DAY(EOMONTH(J14, 0))</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N22" s="1">
         <v>1500</v>
@@ -3809,7 +3809,7 @@
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N23" s="1">
         <v>1800</v>
@@ -3836,7 +3836,7 @@
       </c>
       <c r="J25" s="56">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>200</v>
+        <v>20</v>
       </c>
       <c r="M25" s="68" t="s">
         <v>37</v>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="J26" s="57">
         <f>MAX(0,C9-J25)</f>
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="M26" s="16" t="s">
         <v>9</v>
@@ -3876,7 +3876,7 @@
       </c>
       <c r="J27" s="54">
         <f t="array" ref="J27">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J26))</f>
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="M27" s="34">
         <v>0</v>
@@ -3924,7 +3924,7 @@
       </c>
       <c r="J29" s="61">
         <f>J8</f>
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="M29" s="40">
         <v>1600</v>
@@ -3948,7 +3948,7 @@
       </c>
       <c r="J30" s="60">
         <f>J29*J28</f>
-        <v>1029</v>
+        <v>0</v>
       </c>
       <c r="M30" s="43">
         <v>2200</v>
@@ -3973,7 +3973,7 @@
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="M31" s="47">
         <v>2500</v>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
-        <v>484</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="33" spans="5:10" x14ac:dyDescent="0.25">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="J33" s="6">
         <f>J30+J32</f>
-        <v>1513</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
@@ -4017,7 +4017,7 @@
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
-        <v>2713</v>
+        <v>2520</v>
       </c>
     </row>
   </sheetData>
@@ -4112,8 +4112,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="43" width="8.85546875" style="2" customWidth="1"/>
-    <col min="44" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="44" width="8.85546875" style="2" customWidth="1"/>
+    <col min="45" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4146,7 +4146,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>September 2025</v>
+        <v>October 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>
@@ -4949,8 +4949,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="43" width="8.85546875" style="2" customWidth="1"/>
-    <col min="44" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="44" width="8.85546875" style="2" customWidth="1"/>
+    <col min="45" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4983,7 +4983,7 @@
       </c>
       <c r="E5" s="14" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>September 2025</v>
+        <v>October 2025</v>
       </c>
       <c r="F5" s="14" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Added Oct progress report for pa
</commit_message>
<xml_diff>
--- a/DriveSummaryPython.xlsx
+++ b/DriveSummaryPython.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/DriveDashboardPython/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_827B1A28EC29E536E13BCA8A87AF1E0808C0452D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03019B32-D834-48E8-BB07-1E79455A56B0}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_427DDE56BB5526123A72B3FED2EE9631FC814DB8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{712699E0-2363-4D96-B6A9-C60236951738}"/>
   <bookViews>
-    <workbookView xWindow="2910" yWindow="-16320" windowWidth="19440" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4140" yWindow="-16320" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stefan" sheetId="1" r:id="rId1"/>
@@ -3246,8 +3246,8 @@
   </sheetPr>
   <dimension ref="B2:AC34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3270,8 +3270,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="44" width="8.85546875" style="2" customWidth="1"/>
-    <col min="45" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="45" width="8.85546875" style="2" customWidth="1"/>
+    <col min="46" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4112,8 +4112,8 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="44" width="8.85546875" style="2" customWidth="1"/>
-    <col min="45" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="45" width="8.85546875" style="2" customWidth="1"/>
+    <col min="46" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -4925,8 +4925,8 @@
   </sheetPr>
   <dimension ref="B2:AC34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4949,14 +4949,14 @@
     <col min="19" max="19" width="2.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="9.7109375" style="5" customWidth="1"/>
     <col min="21" max="23" width="9.7109375" style="2" customWidth="1"/>
-    <col min="24" max="44" width="8.85546875" style="2" customWidth="1"/>
-    <col min="45" max="16384" width="8.85546875" style="2"/>
+    <col min="24" max="45" width="8.85546875" style="2" customWidth="1"/>
+    <col min="46" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:29" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="71" t="str">
         <f>_xlfn.CONCAT("Drive Summary ",J13, " ",TEXT(J14, "mmmm yyyy"))</f>
-        <v>Drive Summary Derrick May 2025</v>
+        <v>Drive Summary Derrick October 2025</v>
       </c>
       <c r="C2" s="72"/>
       <c r="D2" s="72"/>
@@ -5020,17 +5020,17 @@
       </c>
       <c r="F6" s="6">
         <f>J9</f>
-        <v>1500</v>
+        <v>1412.046</v>
       </c>
       <c r="G6" s="17">
         <f>J33</f>
-        <v>1392</v>
+        <v>984</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J6" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L6" s="16" t="s">
         <v>9</v>
@@ -5070,17 +5070,17 @@
       </c>
       <c r="F7" s="6">
         <f>F6/J23*J22</f>
-        <v>1660.7142857142856</v>
+        <v>2188.6713</v>
       </c>
       <c r="G7" s="6">
         <f>G6/J23*J22</f>
-        <v>1541.1428571428571</v>
+        <v>1525.2</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J7" s="1">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="L7" s="11">
         <v>0</v>
@@ -5111,24 +5111,24 @@
       </c>
       <c r="C8" s="6">
         <f>300-J7</f>
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="E8" s="10" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="65">
         <f>F6/J23</f>
-        <v>53.571428571428569</v>
+        <v>70.6023</v>
       </c>
       <c r="G8" s="65">
         <f>G6/J23</f>
-        <v>49.714285714285715</v>
+        <v>49.2</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J8" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L8" s="11">
         <v>300</v>
@@ -5158,24 +5158,24 @@
       </c>
       <c r="C9" s="6">
         <f>VLOOKUP(IF(C13,F7,F6),N17:P23,3)</f>
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E9" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="63" t="str">
+      <c r="F9" s="63">
         <f>IF(J27&gt;=M13, "Unlimited", J27-F6)</f>
-        <v>Unlimited</v>
+        <v>386.95399999999995</v>
       </c>
       <c r="G9" s="63">
         <f>50*J24 + IF(J22&lt;30,(30-J22)*G8,0)</f>
-        <v>150</v>
+        <v>550</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="J9" s="1">
-        <v>1500</v>
+        <v>1412.046</v>
       </c>
       <c r="L9" s="11">
         <v>600</v>
@@ -5236,7 +5236,7 @@
       </c>
       <c r="C11" s="6">
         <f>SUM(C6:C10)</f>
-        <v>2600</v>
+        <v>2682</v>
       </c>
       <c r="I11" s="68" t="s">
         <v>25</v>
@@ -5345,7 +5345,7 @@
         <v>30</v>
       </c>
       <c r="J14" s="58">
-        <v>45805</v>
+        <v>45950</v>
       </c>
     </row>
     <row r="15" spans="2:29" x14ac:dyDescent="0.25">
@@ -5407,7 +5407,9 @@
       <c r="I18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="J18" s="1"/>
+      <c r="J18" s="1">
+        <v>50</v>
+      </c>
       <c r="N18" s="1">
         <v>300</v>
       </c>
@@ -5464,7 +5466,7 @@
     <row r="22" spans="9:17" x14ac:dyDescent="0.25">
       <c r="I22" s="52" t="str">
         <f>_xlfn.CONCAT("Days ",TEXT(J14, "mmm yyyy"))</f>
-        <v>Days May 2025</v>
+        <v>Days Oct 2025</v>
       </c>
       <c r="J22" s="55">
         <f>DAY(EOMONTH(J14, 0))</f>
@@ -5486,7 +5488,7 @@
       </c>
       <c r="J23" s="55">
         <f>DAY(J14)</f>
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="N23" s="1">
         <v>1800</v>
@@ -5504,7 +5506,7 @@
       </c>
       <c r="J24" s="54">
         <f>J22-J23</f>
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="9:17" x14ac:dyDescent="0.25">
@@ -5513,7 +5515,7 @@
       </c>
       <c r="J25" s="56">
         <f>C11-VLOOKUP(C11,M27:O31,1,TRUE)</f>
-        <v>100</v>
+        <v>182</v>
       </c>
       <c r="M25" s="68" t="s">
         <v>37</v>
@@ -5529,7 +5531,7 @@
       </c>
       <c r="J26" s="57">
         <f>MAX(0,C9-J25)</f>
-        <v>100</v>
+        <v>118</v>
       </c>
       <c r="M26" s="16" t="s">
         <v>9</v>
@@ -5553,7 +5555,7 @@
       </c>
       <c r="J27" s="54">
         <f t="array" ref="J27">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(O17),_xlfn.ANCHORARRAY( P17)&gt;=J26))</f>
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="M27" s="34">
         <v>0</v>
@@ -5601,7 +5603,7 @@
       </c>
       <c r="J29" s="61">
         <f>J8</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M29" s="40">
         <v>1600</v>
@@ -5625,7 +5627,7 @@
       </c>
       <c r="J30" s="60">
         <f>J29*J28</f>
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="M30" s="43">
         <v>2200</v>
@@ -5649,7 +5651,7 @@
       </c>
       <c r="J31" s="53">
         <f>J23-J29</f>
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="M31" s="47">
         <v>2500</v>
@@ -5673,7 +5675,7 @@
       </c>
       <c r="J32" s="59">
         <f>50*J31-J6</f>
-        <v>1192</v>
+        <v>984</v>
       </c>
     </row>
     <row r="33" spans="9:10" x14ac:dyDescent="0.25">
@@ -5682,7 +5684,7 @@
       </c>
       <c r="J33" s="6">
         <f>J30+J32</f>
-        <v>1392</v>
+        <v>984</v>
       </c>
     </row>
     <row r="34" spans="9:10" x14ac:dyDescent="0.25">
@@ -5691,7 +5693,7 @@
       </c>
       <c r="J34" s="6">
         <f>J33+SUM(C7:C10)</f>
-        <v>2492</v>
+        <v>2166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>